<commit_message>
Finalizando o projeto - Incluido tratamento de erros, seleção e loop dentro de pasta
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -1358,6 +1358,1854 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E27" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E28" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E29" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E30" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E31" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E32" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E33" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E34" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E35" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E36" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E37" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E38" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E39" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E40" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E41" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E42" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E43" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E44" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E45" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E46" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E47" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E48" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E49" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E50" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E51" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E52" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E53" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E54" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E55" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E56" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E57" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E58" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E59" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E60" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E61" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E62" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>24182</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>PEITO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>3850</v>
+      </c>
+      <c r="E63" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>24183</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>PALETA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>7150</v>
+      </c>
+      <c r="E64" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>24184</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>PESCOCO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E65" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>24185</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>PEIXINHO</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E66" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>24186</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>MUSCULO</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2750</v>
+      </c>
+      <c r="E67" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>BM 558/2025</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>24188</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ACEM</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>6330</v>
+      </c>
+      <c r="E68" t="n">
+        <v>27500</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>HUNAN PILOT INTERNATIONAL TRADE CO.,LTD</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>REP. POPULAR DA CHINA</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>24 MONTHS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>